<commit_message>
Handle object creation and format on formulas
</commit_message>
<xml_diff>
--- a/caplet_test.xlsx
+++ b/caplet_test.xlsx
@@ -16,7 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+  <si>
+    <t xml:space="preserve">Summary
+</t>
+  </si>
   <si>
     <t xml:space="preserve">The following sheet demonstrates creating a QuantSA zero curve and 
 </t>
@@ -48,41 +52,32 @@
     <t>dates</t>
   </si>
   <si>
-    <t>2018-07-27</t>
+    <t>continuousRates</t>
   </si>
   <si>
     <t xml:space="preserve">Caplet
 </t>
   </si>
   <si>
-    <t>2019-07-27</t>
-  </si>
-  <si>
     <t>callOrPut</t>
   </si>
   <si>
-    <t>2020-07-27</t>
+    <t>Call</t>
   </si>
   <si>
     <t>strike</t>
   </si>
   <si>
-    <t>[endtable_c]</t>
-  </si>
-  <si>
     <t>notional</t>
   </si>
   <si>
+    <t>zarCurve</t>
+  </si>
+  <si>
     <t>exerciseDate</t>
   </si>
   <si>
-    <t>[create_h]</t>
-  </si>
-  <si>
     <t>settlementDate</t>
-  </si>
-  <si>
-    <t>zarCurve</t>
   </si>
   <si>
     <t>accrueStartDate</t>
@@ -131,20 +126,20 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <b val="1"/>
+      <strike val="0"/>
+      <color rgb="FF000000"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <i val="1"/>
       <strike val="0"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <strike val="0"/>
-      <color rgb="FF000000"/>
-      <sz val="16"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -175,6 +170,18 @@
         <bgColor rgb="FFD8E4BC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFABF8F"/>
+        <bgColor rgb="FFFABF8F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD5B4"/>
+        <bgColor rgb="FFFCD5B4"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -188,15 +195,19 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="4" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="4" fontId="0" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="4" fontId="0" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="5" fontId="0" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="5" fontId="0" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -494,7 +505,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A7"/>
+  <dimension ref="B2:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,37 +513,42 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="100"/>
+    <col customWidth="1" max="2" min="2" width="100"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2">
+      <c r="B8" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -546,7 +562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H21"/>
+  <dimension ref="B2:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,185 +570,181 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:8">
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="n">
+    <row r="2" spans="1:6">
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="n">
         <v>43308</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="4" t="n"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="G3" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="5" t="n">
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="E3" s="4" t="n">
+        <v>43308</v>
+      </c>
+      <c r="F3" s="5" t="n">
         <v>0.07099999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
+    <row r="4" spans="1:6">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="E4" s="4" t="n">
+        <v>43673</v>
+      </c>
+      <c r="F4" s="5" t="n">
         <v>0.07200000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:6">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="n"/>
-      <c r="G5" s="2" t="s">
+      <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="E5" s="4" t="n">
+        <v>44039</v>
+      </c>
+      <c r="F5" s="5" t="n">
         <v>0.073</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:6">
+      <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0.07000000000000001</v>
       </c>
-      <c r="G6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="4" t="n"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="7" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="4" t="n"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="B8" s="2" t="s">
+      <c r="F7" s="9">
+        <f>QSA.CreateDatesAndRatesCurve(E7,E3:E5,F3:F5)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="4" t="n">
         <v>43400</v>
       </c>
-      <c r="G8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="4" t="n"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="4" t="n">
+        <v>43400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C10" s="4" t="n">
         <v>43400</v>
       </c>
-      <c r="G9" s="2" t="s">
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="7">
-        <f>QSA.CreateDatesAndRatesCurve("name",H2,continuousRates)
-</f>
+      <c r="C11" s="4" t="n">
+        <v>43492</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="10">
+        <f>C16</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="3" t="n">
-        <v>43400</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="B11" s="2" t="s">
+    <row r="15" spans="1:6">
+      <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="3" t="n">
-        <v>43492</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="B13" s="6" t="s">
+      <c r="C15" s="11">
+        <f>QSA.GetYearFraction(C2,C9,"ACT365")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="7">
-        <f>C17
-</f>
+      <c r="C16" s="10">
+        <f>QSA.GetSimpleForward(F7,C10,C11)</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="B15" s="2" t="s">
+    <row r="17" spans="1:6">
+      <c r="B17" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" s="7">
-        <f>QSA.GetYearFraction(C2,C9,"ACT365")
-</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="B16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="7">
-        <f>QSA.GetSimpleForward(zarCurve,C10,C11)
-</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="B17" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C17" s="5" t="n">
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="B18" s="2" t="s">
+    <row r="18" spans="1:6">
+      <c r="B18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="11">
+        <f>QSA.GetDF(F7,C9)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="11">
+        <f>QSA.GetYearFraction(C10,C11)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="B21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="7">
-        <f>QSA.GetDF(zarCurve,C9)
-</f>
+      <c r="C21" s="11">
+        <f>1000000*C19*QSA.FormulaBlack(C5,C14,C15,C16,C17,C18)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="7">
-        <f>QSA.GetYearFraction(C10,C11)
-</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="B21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="7">
-        <f>1000000*accrualFraction*QSA.FormulaBlack(C5,C6,timeToExercise,forward,C17,discountfactor)
-</f>
-        <v/>
-      </c>
-    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="C5" type="list">
+      <formula1>"Call,Put"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>